<commit_message>
added padding for USL and LSL
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Om.Parmar\Downloads\Type-1-Gauge-Study-with-Python-main\Type-1-Gauge-Study-with-Python-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ompar\Desktop\Capability-Script\Type-1-Gauge-Study-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D7CF3A-87B9-4F6A-B671-1C529ABA5D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71C79EF-12A2-4B25-9D86-4FB51540AB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7DA59FF9-FCB1-439F-A5ED-7800F04EB215}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{AB7805FB-45E8-43CC-9969-528674049998}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Distance</t>
+    <t>Pat Score</t>
   </si>
   <si>
-    <t>Distance1</t>
+    <t>Pat Scale</t>
+  </si>
+  <si>
+    <t>Blob Area</t>
+  </si>
+  <si>
+    <t>Circle Radius</t>
   </si>
   <si>
     <t>Index</t>
@@ -55,7 +61,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -110,39 +116,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -194,7 +200,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -305,13 +311,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -320,6 +319,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -384,29 +390,49 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252D08A1-2AB0-4B4B-B603-8FBFEE70370C}">
-  <dimension ref="A1:E53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC78907-CF97-4160-BAE0-CBE5437E8184}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -415,10 +441,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -426,16 +452,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>78.659223736811995</v>
+        <v>0.98686486482620195</v>
       </c>
       <c r="C2">
-        <v>76.724072609116703</v>
+        <v>0.98237822634665395</v>
       </c>
       <c r="D2">
-        <v>216.31857091024301</v>
+        <v>169.00000000000099</v>
       </c>
       <c r="E2">
-        <v>174.92412788390001</v>
+        <v>470.0758480028</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -443,16 +469,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>79.1595679541566</v>
+        <v>0.98484873771667503</v>
       </c>
       <c r="C3">
-        <v>77.288930756804405</v>
+        <v>0.98243540347110603</v>
       </c>
       <c r="D3">
-        <v>215.826334692568</v>
+        <v>168.00000000000099</v>
       </c>
       <c r="E3">
-        <v>174.31362588480201</v>
+        <v>470.44874928163301</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -460,16 +486,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>79.849257443340207</v>
+        <v>0.98283261060714699</v>
       </c>
       <c r="C4">
-        <v>76.897601531388901</v>
+        <v>0.98187785575750697</v>
       </c>
       <c r="D4">
-        <v>215.599832517273</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E4">
-        <v>174.49208996453601</v>
+        <v>471.28535279054501</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -477,16 +503,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>78.821486652261896</v>
+        <v>0.98535275459289595</v>
       </c>
       <c r="C5">
-        <v>77.017214523372104</v>
+        <v>0.98183511605514695</v>
       </c>
       <c r="D5">
-        <v>215.775032566752</v>
+        <v>166.00000000000099</v>
       </c>
       <c r="E5">
-        <v>174.94723133278401</v>
+        <v>471.29069818968998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -494,16 +520,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>80.556930330342695</v>
+        <v>0.98686486482620195</v>
       </c>
       <c r="C6">
-        <v>76.942097978839897</v>
+        <v>0.98239296976609602</v>
       </c>
       <c r="D6">
-        <v>217.24544786897701</v>
+        <v>169.00000000000099</v>
       </c>
       <c r="E6">
-        <v>186.93895026560699</v>
+        <v>470.06197129022701</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -511,16 +537,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>80.294102989636201</v>
+        <v>0.98535275459289595</v>
       </c>
       <c r="C7">
-        <v>76.836889770648895</v>
+        <v>0.98238923942171297</v>
       </c>
       <c r="D7">
-        <v>214.83725349195899</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E7">
-        <v>173.55823003345699</v>
+        <v>470.50705386179698</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -528,16 +554,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>79.424204416536497</v>
+        <v>0.98472100496292103</v>
       </c>
       <c r="C8">
-        <v>76.9805019306378</v>
+        <v>0.98190905516316196</v>
       </c>
       <c r="D8">
-        <v>210.419807482279</v>
+        <v>166.00000000000099</v>
       </c>
       <c r="E8">
-        <v>185.70263997334601</v>
+        <v>471.31707426793702</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,16 +571,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>79.699103004658696</v>
+        <v>0.98686486482620195</v>
       </c>
       <c r="C9">
-        <v>77.067854882915498</v>
+        <v>0.98245251075972195</v>
       </c>
       <c r="D9">
-        <v>214.36389894211101</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E9">
-        <v>174.07675059134701</v>
+        <v>470.07449700180001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -562,16 +588,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>79.600678439151494</v>
+        <v>0.98294484615325906</v>
       </c>
       <c r="C10">
-        <v>77.010903483177898</v>
+        <v>0.98237265700116005</v>
       </c>
       <c r="D10">
-        <v>213.88444199428301</v>
+        <v>168.00000000000099</v>
       </c>
       <c r="E10">
-        <v>172.469608185086</v>
+        <v>470.953069110218</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -579,16 +605,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>79.304694891582798</v>
+        <v>0.98434472084045399</v>
       </c>
       <c r="C11">
-        <v>76.990742167356004</v>
+        <v>0.98242028099679801</v>
       </c>
       <c r="D11">
-        <v>214.71499165327401</v>
+        <v>165.00000000000099</v>
       </c>
       <c r="E11">
-        <v>173.62102222898699</v>
+        <v>470.77642242236902</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -596,16 +622,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>79.9648834349846</v>
+        <v>0.98251760005950906</v>
       </c>
       <c r="C12">
-        <v>77.469282317369206</v>
+        <v>0.98235897242137105</v>
       </c>
       <c r="D12">
-        <v>214.32752963816799</v>
+        <v>166.00000000000099</v>
       </c>
       <c r="E12">
-        <v>172.86379036036999</v>
+        <v>470.64754984265801</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,16 +639,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>80.098622680056806</v>
+        <v>0.98862558603286699</v>
       </c>
       <c r="C13">
-        <v>77.441457978799306</v>
+        <v>0.98242973248116705</v>
       </c>
       <c r="D13">
-        <v>213.89917339780399</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E13">
-        <v>172.17980097476101</v>
+        <v>469.89903497652301</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -630,16 +656,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>79.371010202155901</v>
+        <v>0.98609846830367998</v>
       </c>
       <c r="C14">
-        <v>77.355537314422904</v>
+        <v>0.982324605456389</v>
       </c>
       <c r="D14">
-        <v>213.93894941722601</v>
+        <v>171.00000000000099</v>
       </c>
       <c r="E14">
-        <v>172.689375030245</v>
+        <v>470.037400040894</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -647,16 +673,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>79.503580314652794</v>
+        <v>0.98228567838668801</v>
       </c>
       <c r="C15">
-        <v>77.323330736588105</v>
+        <v>0.98214407594290698</v>
       </c>
       <c r="D15">
-        <v>215.083275900384</v>
+        <v>169.00000000000099</v>
       </c>
       <c r="E15">
-        <v>184.49499995990899</v>
+        <v>470.442230297273</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -664,16 +690,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>79.587388631945998</v>
+        <v>0.98709160089492798</v>
       </c>
       <c r="C16">
-        <v>77.437545075339699</v>
+        <v>0.98203525632079602</v>
       </c>
       <c r="D16">
-        <v>210.05771827119401</v>
+        <v>166.00000000000099</v>
       </c>
       <c r="E16">
-        <v>184.630506427076</v>
+        <v>469.93217921837697</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -681,16 +707,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>79.277393528277798</v>
+        <v>0.98439186811447099</v>
       </c>
       <c r="C17">
-        <v>77.093261573101898</v>
+        <v>0.98243393031459303</v>
       </c>
       <c r="D17">
-        <v>210.59418569355799</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E17">
-        <v>184.93860615554999</v>
+        <v>470.06426331976598</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -698,16 +724,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>79.051202701028103</v>
+        <v>0.98199820518493697</v>
       </c>
       <c r="C18">
-        <v>76.990935840348996</v>
+        <v>0.98242357460018304</v>
       </c>
       <c r="D18">
-        <v>209.784261400811</v>
+        <v>166.00000000000099</v>
       </c>
       <c r="E18">
-        <v>184.21433344823501</v>
+        <v>470.430853554279</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -715,16 +741,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>79.553657578817905</v>
+        <v>0.98686486482620195</v>
       </c>
       <c r="C19">
-        <v>77.243291317320597</v>
+        <v>0.98248927834729005</v>
       </c>
       <c r="D19">
-        <v>213.91709194286199</v>
+        <v>164.00000000000099</v>
       </c>
       <c r="E19">
-        <v>172.826211646117</v>
+        <v>470.07692579815102</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -732,379 +758,203 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>79.695496606304204</v>
+        <v>0.98230338096618697</v>
       </c>
       <c r="C20">
-        <v>77.057156117134795</v>
+        <v>0.98206534386856204</v>
       </c>
       <c r="D20">
-        <v>214.16086280519301</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E20">
-        <v>183.94671386243601</v>
+        <v>469.92216589420298</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21">
+        <v>0.98113006353378296</v>
+      </c>
+      <c r="C21">
+        <v>0.98242314459387703</v>
+      </c>
       <c r="D21">
-        <v>208.70695499783901</v>
+        <v>165.00000000000099</v>
       </c>
       <c r="E21">
-        <v>183.47485357409099</v>
+        <v>470.50249706575698</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22">
+        <v>0.98597764968872104</v>
+      </c>
+      <c r="C22">
+        <v>0.98246243699598801</v>
+      </c>
       <c r="D22">
-        <v>215.36660789341701</v>
+        <v>164.00000000000099</v>
       </c>
       <c r="E22">
-        <v>174.01326981438299</v>
+        <v>470.53635723263397</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23">
+        <v>0.98332327604293801</v>
+      </c>
+      <c r="C23">
+        <v>0.98247125390342105</v>
+      </c>
       <c r="D23">
-        <v>213.430214623712</v>
+        <v>166.00000000000099</v>
       </c>
       <c r="E23">
-        <v>172.64089208629801</v>
+        <v>470.44664167721498</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24">
+        <v>0.9806769490242</v>
+      </c>
+      <c r="C24">
+        <v>0.98192207291900602</v>
+      </c>
       <c r="D24">
-        <v>156.91783743046699</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E24">
-        <v>117.704823605168</v>
+        <v>471.29625183433001</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25">
+        <v>0.98849779367446899</v>
+      </c>
+      <c r="C25">
+        <v>0.98235661607176605</v>
+      </c>
       <c r="D25">
-        <v>157.86647782311701</v>
+        <v>166.00000000000099</v>
       </c>
       <c r="E25">
-        <v>117.867818176184</v>
+        <v>470.063339296989</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26">
+        <v>0.98972958326339699</v>
+      </c>
+      <c r="C26">
+        <v>0.98210168907657802</v>
+      </c>
       <c r="D26">
-        <v>157.06377942136399</v>
+        <v>169.00000000000099</v>
       </c>
       <c r="E26">
-        <v>116.86978775075799</v>
+        <v>470.80782482651</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27">
+        <v>0.98535275459289595</v>
+      </c>
+      <c r="C27">
+        <v>0.98242096723447803</v>
+      </c>
       <c r="D27">
-        <v>158.60215321069299</v>
+        <v>168.00000000000099</v>
       </c>
       <c r="E27">
-        <v>118.183283762736</v>
+        <v>470.93816068362202</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28">
+        <v>0.98535275459289595</v>
+      </c>
+      <c r="C28">
+        <v>0.98230112608531694</v>
+      </c>
       <c r="D28">
-        <v>159.47903306040601</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E28">
-        <v>119.389740951723</v>
+        <v>470.51287874515498</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29">
+        <v>0.98861849308013905</v>
+      </c>
+      <c r="C29">
+        <v>0.98254399655283298</v>
+      </c>
       <c r="D29">
-        <v>157.84190408755501</v>
+        <v>166.00000000000099</v>
       </c>
       <c r="E29">
-        <v>117.97181267443</v>
+        <v>470.93788420214901</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30">
+        <v>0.989005327224731</v>
+      </c>
+      <c r="C30">
+        <v>0.98189669255020495</v>
+      </c>
       <c r="D30">
-        <v>157.68592073889101</v>
+        <v>169.00000000000099</v>
       </c>
       <c r="E30">
-        <v>118.022595584492</v>
+        <v>470.88103718091003</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31">
+        <v>0.98845964670181297</v>
+      </c>
+      <c r="C31">
+        <v>0.981866395337748</v>
+      </c>
       <c r="D31">
-        <v>158.02399428408901</v>
+        <v>167.00000000000099</v>
       </c>
       <c r="E31">
-        <v>117.977440863379</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="D32">
-        <v>157.571790903264</v>
-      </c>
-      <c r="E32">
-        <v>118.09156136826</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="D33">
-        <v>158.29664785348999</v>
-      </c>
-      <c r="E33">
-        <v>118.67744722462101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="D34">
-        <v>157.908933276656</v>
-      </c>
-      <c r="E34">
-        <v>118.160736198122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="D35">
-        <v>158.06855657072001</v>
-      </c>
-      <c r="E35">
-        <v>117.989468898233</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="D36">
-        <v>158.393332662425</v>
-      </c>
-      <c r="E36">
-        <v>117.75645104336699</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="D37">
-        <v>157.42300655848001</v>
-      </c>
-      <c r="E37">
-        <v>117.251024139229</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="D38">
-        <v>157.40666914321699</v>
-      </c>
-      <c r="E38">
-        <v>117.6470132922</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="D39">
-        <v>120.31366209699399</v>
-      </c>
-      <c r="E39">
-        <v>94.111570386222297</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="D40">
-        <v>120.60208252891999</v>
-      </c>
-      <c r="E40">
-        <v>94.350552115910901</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="D41">
-        <v>119.982431845962</v>
-      </c>
-      <c r="E41">
-        <v>94.758342284337104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="D42">
-        <v>119.938594139584</v>
-      </c>
-      <c r="E42">
-        <v>94.425021445035</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="D43">
-        <v>119.249596158527</v>
-      </c>
-      <c r="E43">
-        <v>93.820365306007602</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="D44">
-        <v>122.068921459145</v>
-      </c>
-      <c r="E44">
-        <v>95.720853312158894</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="D45">
-        <v>120.47360198389499</v>
-      </c>
-      <c r="E45">
-        <v>94.8938058011273</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="D46">
-        <v>119.89547150355</v>
-      </c>
-      <c r="E46">
-        <v>94.218631920942002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="D47">
-        <v>120.401918812262</v>
-      </c>
-      <c r="E47">
-        <v>94.7793411930286</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="D48">
-        <v>121.570456890231</v>
-      </c>
-      <c r="E48">
-        <v>94.063049726952102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="D49">
-        <v>121.991532837901</v>
-      </c>
-      <c r="E49">
-        <v>95.764810171533099</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="D50">
-        <v>120.38698628001301</v>
-      </c>
-      <c r="E50">
-        <v>94.614940106095204</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="D51">
-        <v>119.93412390627699</v>
-      </c>
-      <c r="E51">
-        <v>94.407136231415294</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="D52">
-        <v>121.77022666643801</v>
-      </c>
-      <c r="E52">
-        <v>95.9536015020701</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="D53">
-        <v>120.443408836141</v>
-      </c>
-      <c r="E53">
-        <v>94.8919987885116</v>
+        <v>471.76189437892901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
quality of life update
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ompar\Desktop\Capability-Script\Type-1-Gauge-Study-with-Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Om.Parmar\Desktop\Type-1-Gauge-Study-with-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71C79EF-12A2-4B25-9D86-4FB51540AB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B820EB-BB4F-4D2B-96E7-877BCCB5B92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{AB7805FB-45E8-43CC-9969-528674049998}"/>
+    <workbookView xWindow="30" yWindow="750" windowWidth="28770" windowHeight="15450" xr2:uid="{AB7805FB-45E8-43CC-9969-528674049998}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Pat Score</t>
   </si>
@@ -44,13 +44,10 @@
     <t>Pat Scale</t>
   </si>
   <si>
-    <t>Blob Area</t>
+    <t>Index</t>
   </si>
   <si>
-    <t>Circle Radius</t>
-  </si>
-  <si>
-    <t>Index</t>
+    <t>Pat Angle</t>
   </si>
 </sst>
 </file>
@@ -422,539 +419,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC78907-CF97-4160-BAE0-CBE5437E8184}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.98686486482620195</v>
+        <v>0.99767976999999997</v>
       </c>
       <c r="C2">
-        <v>0.98237822634665395</v>
+        <v>1.006922659</v>
       </c>
       <c r="D2">
-        <v>169.00000000000099</v>
-      </c>
-      <c r="E2">
-        <v>470.0758480028</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000488007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.98484873771667503</v>
+        <v>0.99766081600000001</v>
       </c>
       <c r="C3">
-        <v>0.98243540347110603</v>
+        <v>1.0106113889999999</v>
       </c>
       <c r="D3">
-        <v>168.00000000000099</v>
-      </c>
-      <c r="E3">
-        <v>470.44874928163301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0004934569999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.98283261060714699</v>
+        <v>0.99798792599999997</v>
       </c>
       <c r="C4">
-        <v>0.98187785575750697</v>
+        <v>1.011051894</v>
       </c>
       <c r="D4">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E4">
-        <v>471.28535279054501</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0004530979999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.98535275459289595</v>
+        <v>0.99780780099999999</v>
       </c>
       <c r="C5">
-        <v>0.98183511605514695</v>
+        <v>1.011846238</v>
       </c>
       <c r="D5">
-        <v>166.00000000000099</v>
-      </c>
-      <c r="E5">
-        <v>471.29069818968998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0005636899999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.98686486482620195</v>
+        <v>0.99759447599999995</v>
       </c>
       <c r="C6">
-        <v>0.98239296976609602</v>
+        <v>1.0043240040000001</v>
       </c>
       <c r="D6">
-        <v>169.00000000000099</v>
-      </c>
-      <c r="E6">
-        <v>470.06197129022701</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0005371569999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.98535275459289595</v>
+        <v>0.99769872400000004</v>
       </c>
       <c r="C7">
-        <v>0.98238923942171297</v>
+        <v>1.008159475</v>
       </c>
       <c r="D7">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E7">
-        <v>470.50705386179698</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0006020259999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.98472100496292103</v>
+        <v>0.99784094099999998</v>
       </c>
       <c r="C8">
-        <v>0.98190905516316196</v>
+        <v>1.0107334020000001</v>
       </c>
       <c r="D8">
-        <v>166.00000000000099</v>
-      </c>
-      <c r="E8">
-        <v>471.31707426793702</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0006786640000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.98686486482620195</v>
+        <v>0.99776035500000004</v>
       </c>
       <c r="C9">
-        <v>0.98245251075972195</v>
+        <v>1.0139124960000001</v>
       </c>
       <c r="D9">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E9">
-        <v>470.07449700180001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0007625529999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.98294484615325906</v>
+        <v>0.99758022999999996</v>
       </c>
       <c r="C10">
-        <v>0.98237265700116005</v>
+        <v>1.0195471460000001</v>
       </c>
       <c r="D10">
-        <v>168.00000000000099</v>
-      </c>
-      <c r="E10">
-        <v>470.953069110218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000736219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.98434472084045399</v>
+        <v>0.99782675499999995</v>
       </c>
       <c r="C11">
-        <v>0.98242028099679801</v>
+        <v>1.009096019</v>
       </c>
       <c r="D11">
-        <v>165.00000000000099</v>
-      </c>
-      <c r="E11">
-        <v>470.77642242236902</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0005950889999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.98251760005950906</v>
+        <v>0.99748539899999999</v>
       </c>
       <c r="C12">
-        <v>0.98235897242137105</v>
+        <v>1.010877437</v>
       </c>
       <c r="D12">
-        <v>166.00000000000099</v>
-      </c>
-      <c r="E12">
-        <v>470.64754984265801</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0005228900000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.98862558603286699</v>
+        <v>0.99751383100000002</v>
       </c>
       <c r="C13">
-        <v>0.98242973248116705</v>
+        <v>1.026896126</v>
       </c>
       <c r="D13">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E13">
-        <v>469.89903497652301</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0007314490000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.98609846830367998</v>
+        <v>0.99742853600000003</v>
       </c>
       <c r="C14">
-        <v>0.982324605456389</v>
+        <v>1.0194309109999999</v>
       </c>
       <c r="D14">
-        <v>171.00000000000099</v>
-      </c>
-      <c r="E14">
-        <v>470.037400040894</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0007074419999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.98228567838668801</v>
+        <v>0.99789786300000005</v>
       </c>
       <c r="C15">
-        <v>0.98214407594290698</v>
+        <v>1.0066947260000001</v>
       </c>
       <c r="D15">
-        <v>169.00000000000099</v>
-      </c>
-      <c r="E15">
-        <v>470.442230297273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0005827810000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.98709160089492798</v>
+        <v>0.99774140099999997</v>
       </c>
       <c r="C16">
-        <v>0.98203525632079602</v>
+        <v>1.0070822319999999</v>
       </c>
       <c r="D16">
-        <v>166.00000000000099</v>
-      </c>
-      <c r="E16">
-        <v>469.93217921837697</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.00041818</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.98439186811447099</v>
+        <v>0.99766558400000005</v>
       </c>
       <c r="C17">
-        <v>0.98243393031459303</v>
+        <v>1.0066743410000001</v>
       </c>
       <c r="D17">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E17">
-        <v>470.06426331976598</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0004245380000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.98199820518493697</v>
+        <v>0.99748068999999995</v>
       </c>
       <c r="C18">
-        <v>0.98242357460018304</v>
+        <v>1.015842036</v>
       </c>
       <c r="D18">
-        <v>166.00000000000099</v>
-      </c>
-      <c r="E18">
-        <v>470.430853554279</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000434898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.98686486482620195</v>
+        <v>0.99765604699999999</v>
       </c>
       <c r="C19">
-        <v>0.98248927834729005</v>
+        <v>1.0146240630000001</v>
       </c>
       <c r="D19">
-        <v>164.00000000000099</v>
-      </c>
-      <c r="E19">
-        <v>470.07692579815102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000516433</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.98230338096618697</v>
+        <v>0.99749487599999997</v>
       </c>
       <c r="C20">
-        <v>0.98206534386856204</v>
+        <v>1.0145458970000001</v>
       </c>
       <c r="D20">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E20">
-        <v>469.92216589420298</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000581553</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.98113006353378296</v>
+        <v>0.99764186099999996</v>
       </c>
       <c r="C21">
-        <v>0.98242314459387703</v>
+        <v>1.011313688</v>
       </c>
       <c r="D21">
-        <v>165.00000000000099</v>
-      </c>
-      <c r="E21">
-        <v>470.50249706575698</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000508325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.98597764968872104</v>
+        <v>0.99774140099999997</v>
       </c>
       <c r="C22">
-        <v>0.98246243699598801</v>
+        <v>1.0187560870000001</v>
       </c>
       <c r="D22">
-        <v>164.00000000000099</v>
-      </c>
-      <c r="E22">
-        <v>470.53635723263397</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0006578429999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.98332327604293801</v>
+        <v>0.99303871399999999</v>
       </c>
       <c r="C23">
-        <v>0.98247125390342105</v>
+        <v>1.014581841</v>
       </c>
       <c r="D23">
-        <v>166.00000000000099</v>
-      </c>
-      <c r="E23">
-        <v>470.44664167721498</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0007093979999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.9806769490242</v>
+        <v>0.99773669200000004</v>
       </c>
       <c r="C24">
-        <v>0.98192207291900602</v>
+        <v>1.0148323050000001</v>
       </c>
       <c r="D24">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E24">
-        <v>471.29625183433001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000695457</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.98849779367446899</v>
+        <v>0.99304348200000003</v>
       </c>
       <c r="C25">
-        <v>0.98235661607176605</v>
+        <v>1.0228865119999999</v>
       </c>
       <c r="D25">
-        <v>166.00000000000099</v>
-      </c>
-      <c r="E25">
-        <v>470.063339296989</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000730321</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.98972958326339699</v>
+        <v>0.99302452799999996</v>
       </c>
       <c r="C26">
-        <v>0.98210168907657802</v>
+        <v>1.019384831</v>
       </c>
       <c r="D26">
-        <v>169.00000000000099</v>
-      </c>
-      <c r="E26">
-        <v>470.80782482651</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0006223839999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.98535275459289595</v>
+        <v>0.99765604699999999</v>
       </c>
       <c r="C27">
-        <v>0.98242096723447803</v>
+        <v>1.012584946</v>
       </c>
       <c r="D27">
-        <v>168.00000000000099</v>
-      </c>
-      <c r="E27">
-        <v>470.93816068362202</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000390984</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0.98535275459289595</v>
+        <v>0.99757075299999998</v>
       </c>
       <c r="C28">
-        <v>0.98230112608531694</v>
+        <v>1.024532631</v>
       </c>
       <c r="D28">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E28">
-        <v>470.51287874515498</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000533581</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.98861849308013905</v>
+        <v>0.99767029299999999</v>
       </c>
       <c r="C29">
-        <v>0.98254399655283298</v>
+        <v>1.0127353290000001</v>
       </c>
       <c r="D29">
-        <v>166.00000000000099</v>
-      </c>
-      <c r="E29">
-        <v>470.93788420214901</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.000730108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0.989005327224731</v>
+        <v>0.99769401599999996</v>
       </c>
       <c r="C30">
-        <v>0.98189669255020495</v>
+        <v>1.0266902870000001</v>
       </c>
       <c r="D30">
-        <v>169.00000000000099</v>
-      </c>
-      <c r="E30">
-        <v>470.88103718091003</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.0005552040000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
-        <v>0.98845964670181297</v>
+        <v>0.99752336699999999</v>
       </c>
       <c r="C31">
-        <v>0.981866395337748</v>
+        <v>1.0202368930000001</v>
       </c>
       <c r="D31">
-        <v>167.00000000000099</v>
-      </c>
-      <c r="E31">
-        <v>471.76189437892901</v>
+        <v>1.00068734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>